<commit_message>
No crew/ship certificates for 2.1
</commit_message>
<xml_diff>
--- a/Code Lists/ToopDocumentTypeIdentifiers-v5.xlsx
+++ b/Code Lists/ToopDocumentTypeIdentifiers-v5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git\toop\Code Lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EE5553-3C15-41BC-A72C-1B2F8EDAEF66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC069F4-9D8B-49BF-B11D-6B5C658C1D61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="4" r:id="rId1"/>
@@ -26,12 +26,12 @@
     <definedName name="_ftnref3" localSheetId="0">'Document Type'!$A$3</definedName>
     <definedName name="_ftnref4" localSheetId="0">'Document Type'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>Common Name</t>
   </si>
@@ -174,12 +174,6 @@
     <t>EDM Response 2.0</t>
   </si>
   <si>
-    <t>Ship Certificate Data 2.1</t>
-  </si>
-  <si>
-    <t>Crew Certificate Data 2.1</t>
-  </si>
-  <si>
     <t>Ship Certificate Data 2.0</t>
   </si>
   <si>
@@ -193,12 +187,6 @@
   </si>
   <si>
     <t>EDM Response 2.1</t>
-  </si>
-  <si>
-    <t>CrewCertificate::CREWCERTIFICATE_TYPE::UNSTRUCTURED::toop-edm:v2.1</t>
-  </si>
-  <si>
-    <t>ShipCertificate::SHIPCERTIFICATE_TYPE::UNSTRUCTURED::toop-edm:v2.1</t>
   </si>
   <si>
     <t>QueryResponse::toop-edm:v2.1</t>
@@ -706,11 +694,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,7 +1108,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>42</v>
@@ -1138,7 +1126,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>43</v>
@@ -1156,10 +1144,10 @@
     </row>
     <row r="25" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C25" s="5">
         <v>5</v>
@@ -1171,10 +1159,10 @@
     </row>
     <row r="26" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C26" s="5">
         <v>5</v>
@@ -1186,45 +1174,15 @@
     </row>
     <row r="27" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C27" s="5">
         <v>5</v>
       </c>
       <c r="D27" s="5" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="5">
-        <v>5</v>
-      </c>
-      <c r="D28" s="5" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="5">
-        <v>5</v>
-      </c>
-      <c r="D29" s="5" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>

</xml_diff>